<commit_message>
Update STOCK MANAGEMENT SHEET (2).xlsx
</commit_message>
<xml_diff>
--- a/STOCK MANAGEMENT SHEET (2).xlsx
+++ b/STOCK MANAGEMENT SHEET (2).xlsx
@@ -507,12 +507,12 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color rgb="FF000000"/>
+      <color theme="5"/>
       <name val="Cambria"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -559,6 +559,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -916,13 +922,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8041,8 +8047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A32" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>